<commit_message>
Fix extension manager icon issue
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="360" yWindow="60" windowWidth="18510" windowHeight="13365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CheckList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="71">
   <si>
     <t>VS2010</t>
   </si>
@@ -212,9 +211,6 @@
     <t>When "Allow files not under source-control to be updated" is false files not under source control are not modified</t>
   </si>
   <si>
-    <t>When "Keep modified files open after updates" is true then (a) the file remains open in the IDE (b) user can 'undo' the changes e.g. using control-Z</t>
-  </si>
-  <si>
     <t>GitHub ReadMe.md is generally okay</t>
   </si>
   <si>
@@ -224,10 +220,13 @@
     <t>GitHub ReadMe.md link to VS gallery is okay</t>
   </si>
   <si>
-    <t>TO BE TESTED</t>
-  </si>
-  <si>
     <t>Tools &gt; Extensions and Updates &gt; More information (link to GutHub - defined in Manifest &gt; Metadata &gt; More Info Url)</t>
+  </si>
+  <si>
+    <t>GitHub ReadMe.md images are okay</t>
+  </si>
+  <si>
+    <t>When "Keep modified files open after updates" is true then (a) the file remains open in the IDE (b) user can 'undo' the changes</t>
   </si>
 </sst>
 </file>
@@ -249,7 +248,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,12 +258,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -302,9 +295,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -611,19 +601,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="108.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="106" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.33203125" style="2"/>
@@ -681,26 +671,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -714,19 +704,19 @@
       <c r="B4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -766,19 +756,19 @@
       <c r="B6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -792,19 +782,19 @@
       <c r="B7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1026,19 +1016,19 @@
       <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -1078,19 +1068,19 @@
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -1104,19 +1094,19 @@
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="6" t="s">
+      <c r="C19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
@@ -1156,19 +1146,19 @@
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="C21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1494,19 +1484,19 @@
       <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="6" t="s">
+      <c r="C34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="3" t="s">
@@ -1520,19 +1510,19 @@
       <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="6" t="s">
+      <c r="C35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
@@ -1676,19 +1666,19 @@
       <c r="B41" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="6" t="s">
+      <c r="C41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="3" t="s">
@@ -1702,19 +1692,19 @@
       <c r="B42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="6" t="s">
+      <c r="C42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="3" t="s">
@@ -1728,19 +1718,19 @@
       <c r="B43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="6" t="s">
+      <c r="C43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="3" t="s">
@@ -1754,19 +1744,19 @@
       <c r="B44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="6" t="s">
+      <c r="C44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="3" t="s">
@@ -1780,19 +1770,19 @@
       <c r="B45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="6" t="s">
+      <c r="C45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="3" t="s">
@@ -1806,19 +1796,19 @@
       <c r="B46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="6" t="s">
+      <c r="C46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="3" t="s">
@@ -1832,19 +1822,19 @@
       <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="6" t="s">
+      <c r="C47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="3" t="s">
@@ -1903,30 +1893,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1936,31 +1926,31 @@
       <c r="B51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="6" t="s">
+      <c r="C51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>22</v>
@@ -1977,8 +1967,8 @@
       <c r="G52" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>69</v>
+      <c r="H52" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1986,7 +1976,7 @@
         <v>44</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>22</v>
@@ -2012,7 +2002,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>22</v>
@@ -2029,16 +2019,16 @@
       <c r="G54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>13</v>
+      <c r="H54" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>22</v>
@@ -2064,24 +2054,50 @@
         <v>45</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H56" s="3" t="s">
+      <c r="C57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2089,16 +2105,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added changelog and screen shots, de-duplicate and alpha-sort successfull results messages, bug fix for results dialog not appearing under certain circumstances when rules for multiple solutions exist
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="80">
   <si>
     <t>VS2010</t>
   </si>
@@ -227,6 +227,33 @@
   </si>
   <si>
     <t>When "Keep modified files open after updates" is true then (a) the file remains open in the IDE (b) user can 'undo' the changes</t>
+  </si>
+  <si>
+    <t>Images in Description are okay</t>
+  </si>
+  <si>
+    <t>GitHub ReadMe.md CHANGELOG is okay</t>
+  </si>
+  <si>
+    <t>Success messages are sorted alphabetically</t>
+  </si>
+  <si>
+    <t>Success messages are not duplicated (i.e. 2 rules for same file)</t>
+  </si>
+  <si>
+    <t>When rules exist for different solutions that are enabled-rules, the results dialog is still displayed when opening solution for rule 1</t>
+  </si>
+  <si>
+    <t>GitHub ReadMe.md RELEASENOTES is okay</t>
+  </si>
+  <si>
+    <t>Hyperlinks in Description are okay (github, release notes, changelog)</t>
+  </si>
+  <si>
+    <t>VS Extension Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">release notes, images etc etc etc </t>
   </si>
 </sst>
 </file>
@@ -248,7 +275,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -280,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -295,6 +328,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -601,13 +637,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>22</v>
@@ -1395,8 +1431,8 @@
       <c r="G30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>6</v>
+      <c r="H30" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1404,7 +1440,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>22</v>
@@ -1421,8 +1457,8 @@
       <c r="G31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>6</v>
+      <c r="H31" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1430,7 +1466,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>22</v>
@@ -1455,127 +1491,127 @@
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="C35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="C36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>22</v>
+      <c r="C37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>6</v>
@@ -1585,8 +1621,8 @@
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>56</v>
+      <c r="B38" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>22</v>
@@ -1611,8 +1647,8 @@
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>35</v>
+      <c r="B39" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>22</v>
@@ -1638,7 +1674,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>22</v>
@@ -1661,25 +1697,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>13</v>
+        <v>35</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>6</v>
@@ -1687,54 +1723,54 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1742,7 +1778,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>13</v>
@@ -1768,7 +1804,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>13</v>
@@ -1794,7 +1830,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>13</v>
@@ -1820,7 +1856,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
@@ -1846,22 +1882,22 @@
         <v>43</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>6</v>
@@ -1872,22 +1908,22 @@
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>6</v>
@@ -1898,7 +1934,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>13</v>
@@ -1924,22 +1960,22 @@
         <v>43</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>6</v>
@@ -1947,10 +1983,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>22</v>
@@ -1973,25 +2009,25 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>22</v>
+        <v>68</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>6</v>
@@ -1999,25 +2035,25 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>6</v>
@@ -2028,7 +2064,7 @@
         <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>22</v>
@@ -2051,10 +2087,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>22</v>
@@ -2071,34 +2107,224 @@
       <c r="G56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>6</v>
+      <c r="H56" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>6</v>
+      <c r="C62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug whereby exporting rules as CSV crashes if no rules exist
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\AutoFindReplace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="18510" windowHeight="13365"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="80">
   <si>
     <t>VS2010</t>
   </si>
@@ -130,12 +135,6 @@
     <t>Functionality</t>
   </si>
   <si>
-    <t>Tools &gt; Options &gt; Export rules as JSON works</t>
-  </si>
-  <si>
-    <t>Tools &gt; Options &gt; Export rules as CSV works</t>
-  </si>
-  <si>
     <t>Tools &gt; Options &gt; Rules can be added, and when added they take effect successfully</t>
   </si>
   <si>
@@ -250,10 +249,16 @@
     <t>Hyperlinks in Description are okay (github, release notes, changelog)</t>
   </si>
   <si>
-    <t>VS Extension Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">release notes, images etc etc etc </t>
+    <t>Tools &gt; Options &gt; Export rules as CSV works, when no rules exist</t>
+  </si>
+  <si>
+    <t>Tools &gt; Options &gt; Export rules as JSON works, when no rules exist</t>
+  </si>
+  <si>
+    <t>Tools &gt; Options &gt; Export rules as JSON works, when rules exist</t>
+  </si>
+  <si>
+    <t>Tools &gt; Options &gt; Export rules as CSV works, when rules exist</t>
   </si>
 </sst>
 </file>
@@ -393,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -428,7 +433,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,13 +642,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -657,7 +662,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
@@ -686,7 +691,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
@@ -712,7 +717,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>13</v>
@@ -738,7 +743,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
@@ -764,7 +769,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
@@ -790,7 +795,7 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
@@ -816,7 +821,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -868,7 +873,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
@@ -894,7 +899,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>22</v>
@@ -920,7 +925,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>22</v>
@@ -946,7 +951,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>22</v>
@@ -972,7 +977,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>22</v>
@@ -998,7 +1003,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>22</v>
@@ -1024,7 +1029,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>22</v>
@@ -1050,7 +1055,7 @@
         <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
@@ -1076,22 +1081,22 @@
         <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>22</v>
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>6</v>
@@ -1102,22 +1107,22 @@
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>13</v>
+        <v>79</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>6</v>
@@ -1128,22 +1133,22 @@
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>13</v>
+        <v>76</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>6</v>
@@ -1154,22 +1159,22 @@
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>6</v>
@@ -1180,7 +1185,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>13</v>
@@ -1206,7 +1211,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>22</v>
@@ -1232,22 +1237,22 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>6</v>
@@ -1258,7 +1263,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>22</v>
@@ -1284,7 +1289,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>22</v>
@@ -1310,7 +1315,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>22</v>
@@ -1336,7 +1341,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>22</v>
@@ -1362,7 +1367,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>22</v>
@@ -1388,7 +1393,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>22</v>
@@ -1414,7 +1419,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>22</v>
@@ -1431,8 +1436,8 @@
       <c r="G30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>13</v>
+      <c r="H30" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1440,7 +1445,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>22</v>
@@ -1457,8 +1462,8 @@
       <c r="G31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>13</v>
+      <c r="H31" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1466,7 +1471,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>22</v>
@@ -1492,7 +1497,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
@@ -1518,7 +1523,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>22</v>
@@ -1543,127 +1548,127 @@
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="C38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>22</v>
+      <c r="C39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>6</v>
@@ -1673,8 +1678,8 @@
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>56</v>
+      <c r="B40" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>22</v>
@@ -1699,8 +1704,8 @@
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>35</v>
+      <c r="B41" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>22</v>
@@ -1726,7 +1731,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>22</v>
@@ -1747,12 +1752,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>22</v>
@@ -1769,57 +1774,57 @@
       <c r="G43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>13</v>
+      <c r="H43" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>73</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>6</v>
@@ -1827,10 +1832,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>13</v>
@@ -1847,13 +1852,13 @@
       <c r="G46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>6</v>
+      <c r="H46" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>58</v>
@@ -1873,16 +1878,16 @@
       <c r="G47" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>6</v>
+      <c r="H47" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>13</v>
@@ -1899,16 +1904,16 @@
       <c r="G48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>6</v>
+      <c r="H48" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
@@ -1925,16 +1930,16 @@
       <c r="G49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>6</v>
+      <c r="H49" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>13</v>
@@ -1951,161 +1956,161 @@
       <c r="G50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>6</v>
+      <c r="H50" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>6</v>
+      <c r="C55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>13</v>
@@ -2113,10 +2118,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>22</v>
@@ -2133,16 +2138,16 @@
       <c r="G57" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="6" t="s">
-        <v>13</v>
+      <c r="H57" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>22</v>
@@ -2165,10 +2170,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>22</v>
@@ -2191,10 +2196,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>22</v>
@@ -2217,10 +2222,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>22</v>
@@ -2243,25 +2248,25 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>13</v>
+        <v>65</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>6</v>
@@ -2269,10 +2274,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>22</v>
@@ -2289,42 +2294,86 @@
       <c r="G63" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H63" s="6" t="s">
-        <v>13</v>
+      <c r="H63" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>79</v>
+        <v>43</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ReadMe and ChangeLog enhancements, better message dialog deduplication, better example test rules
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\AutoFindReplace\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="18510" windowHeight="13365"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="82">
   <si>
     <t>VS2010</t>
   </si>
@@ -237,9 +232,6 @@
     <t>Success messages are sorted alphabetically</t>
   </si>
   <si>
-    <t>Success messages are not duplicated (i.e. 2 rules for same file)</t>
-  </si>
-  <si>
     <t>When rules exist for different solutions that are enabled-rules, the results dialog is still displayed when opening solution for rule 1</t>
   </si>
   <si>
@@ -259,6 +251,15 @@
   </si>
   <si>
     <t>Tools &gt; Options &gt; Export rules as CSV works, when rules exist</t>
+  </si>
+  <si>
+    <t>TOTEST</t>
+  </si>
+  <si>
+    <t>Success messages are not duplicated (i.e. 2 rules for same file - with same casing)</t>
+  </si>
+  <si>
+    <t>Success messages are not duplicated (i.e. 2 rules for same file - mixed cases e.g. MyClass.cs &amp; myclass.CS)</t>
   </si>
 </sst>
 </file>
@@ -398,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,13 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1055,7 +1056,7 @@
         <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
@@ -1081,7 +1082,7 @@
         <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>13</v>
@@ -1107,7 +1108,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>22</v>
@@ -1133,7 +1134,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>22</v>
@@ -1497,7 +1498,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
@@ -1523,7 +1524,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>22</v>
@@ -1540,8 +1541,8 @@
       <c r="G34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>6</v>
+      <c r="H34" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1549,7 +1550,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>22</v>
@@ -1575,7 +1576,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>22</v>
@@ -1600,49 +1601,49 @@
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>13</v>
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>6</v>
@@ -1653,48 +1654,48 @@
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>22</v>
+      <c r="C40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>6</v>
@@ -1705,7 +1706,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>22</v>
@@ -1730,8 +1731,8 @@
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>54</v>
+      <c r="B42" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>22</v>
@@ -1757,7 +1758,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>22</v>
@@ -1783,34 +1784,34 @@
         <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C45" s="3" t="s">
         <v>22</v>
       </c>
@@ -1830,30 +1831,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>13</v>
+        <v>72</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1861,7 +1862,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>13</v>
@@ -1887,7 +1888,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>13</v>
@@ -1913,7 +1914,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
@@ -1939,7 +1940,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>13</v>
@@ -1965,7 +1966,7 @@
         <v>41</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
@@ -1991,7 +1992,7 @@
         <v>41</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>13</v>
@@ -2017,22 +2018,22 @@
         <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>13</v>
@@ -2043,7 +2044,7 @@
         <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>22</v>
@@ -2069,22 +2070,22 @@
         <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>13</v>
@@ -2095,7 +2096,7 @@
         <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>13</v>
@@ -2118,28 +2119,28 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2147,7 +2148,7 @@
         <v>42</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>22</v>
@@ -2173,7 +2174,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>22</v>
@@ -2199,7 +2200,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>22</v>
@@ -2225,7 +2226,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>22</v>
@@ -2251,7 +2252,7 @@
         <v>42</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>22</v>
@@ -2274,10 +2275,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>22</v>
@@ -2303,22 +2304,22 @@
         <v>43</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>6</v>
@@ -2329,25 +2330,25 @@
         <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2355,24 +2356,50 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H66" s="6" t="s">
+      <c r="C67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="6" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve results dialog and screen shots
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="81">
   <si>
     <t>VS2010</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>Tools &gt; Options &gt; Export rules as CSV works, when rules exist</t>
-  </si>
-  <si>
-    <t>TOTEST</t>
   </si>
   <si>
     <t>Success messages are not duplicated (i.e. 2 rules for same file - with same casing)</t>
@@ -646,10 +643,10 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1498,7 +1495,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
@@ -1524,7 +1521,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>22</v>
@@ -1541,8 +1538,8 @@
       <c r="G34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>79</v>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Bug fix for a non-text file specified in a rule
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="83">
   <si>
     <t>VS2010</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Success messages are not duplicated (i.e. 2 rules for same file - mixed cases e.g. MyClass.cs &amp; myclass.CS)</t>
+  </si>
+  <si>
+    <t>If opening a solution with a rule for an image file, then nothing is modified &amp; an error is duly reported</t>
+  </si>
+  <si>
+    <t>to be tested</t>
   </si>
 </sst>
 </file>
@@ -640,13 +646,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
+      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1620,53 +1626,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>13</v>
+      <c r="C39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>6</v>
@@ -1677,48 +1683,48 @@
         <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>22</v>
+      <c r="C41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>6</v>
@@ -1729,7 +1735,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>22</v>
@@ -1754,8 +1760,8 @@
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>54</v>
+      <c r="B43" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>22</v>
@@ -1781,7 +1787,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>22</v>
@@ -1807,77 +1813,77 @@
         <v>37</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>13</v>
+      <c r="C47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1885,7 +1891,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>13</v>
@@ -1911,7 +1917,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
@@ -1937,7 +1943,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>13</v>
@@ -1963,7 +1969,7 @@
         <v>41</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>13</v>
@@ -1989,7 +1995,7 @@
         <v>41</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>13</v>
@@ -2015,7 +2021,7 @@
         <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>13</v>
@@ -2041,22 +2047,22 @@
         <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>13</v>
@@ -2067,7 +2073,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>22</v>
@@ -2093,22 +2099,22 @@
         <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>13</v>
@@ -2119,7 +2125,7 @@
         <v>41</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>13</v>
@@ -2142,28 +2148,28 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2171,7 +2177,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>22</v>
@@ -2197,7 +2203,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>22</v>
@@ -2223,7 +2229,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>22</v>
@@ -2249,7 +2255,7 @@
         <v>42</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>22</v>
@@ -2275,7 +2281,7 @@
         <v>42</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>22</v>
@@ -2298,10 +2304,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>22</v>
@@ -2327,22 +2333,22 @@
         <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>6</v>
@@ -2353,25 +2359,25 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2379,24 +2385,50 @@
         <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H67" s="6" t="s">
+      <c r="C68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="6" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor update to test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="82">
   <si>
     <t>VS2010</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>If opening a solution with a rule for an image file, then nothing is modified &amp; an error is duly reported</t>
-  </si>
-  <si>
-    <t>to be tested</t>
   </si>
 </sst>
 </file>
@@ -652,7 +649,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1648,8 +1645,8 @@
       <c r="G38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>82</v>
+      <c r="H38" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Additions to Change Log, updates to Test Cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -281,7 +281,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,12 +300,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -334,9 +328,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -649,7 +640,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomRight" activeCell="H48" sqref="H48:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1905,8 +1896,8 @@
       <c r="G48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="6" t="s">
-        <v>13</v>
+      <c r="H48" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1931,8 +1922,8 @@
       <c r="G49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>13</v>
+      <c r="H49" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1957,8 +1948,8 @@
       <c r="G50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>13</v>
+      <c r="H50" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1983,8 +1974,8 @@
       <c r="G51" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>13</v>
+      <c r="H51" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2009,8 +2000,8 @@
       <c r="G52" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="6" t="s">
-        <v>13</v>
+      <c r="H52" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2035,8 +2026,8 @@
       <c r="G53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="6" t="s">
-        <v>13</v>
+      <c r="H53" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2061,8 +2052,8 @@
       <c r="G54" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="6" t="s">
-        <v>13</v>
+      <c r="H54" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2087,8 +2078,8 @@
       <c r="G55" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H55" s="6" t="s">
-        <v>13</v>
+      <c r="H55" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2113,8 +2104,8 @@
       <c r="G56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="6" t="s">
-        <v>13</v>
+      <c r="H56" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2139,8 +2130,8 @@
       <c r="G57" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H57" s="6" t="s">
-        <v>13</v>
+      <c r="H57" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2165,8 +2156,8 @@
       <c r="G58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H58" s="6" t="s">
-        <v>13</v>
+      <c r="H58" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2399,8 +2390,8 @@
       <c r="G67" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H67" s="6" t="s">
-        <v>13</v>
+      <c r="H67" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2425,8 +2416,8 @@
       <c r="G68" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="6" t="s">
-        <v>13</v>
+      <c r="H68" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case updates and correct line breaks in licence file
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="86">
   <si>
     <t>PASS</t>
   </si>
@@ -265,24 +265,6 @@
   </si>
   <si>
     <t>Basic find / replace works - VS2015</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2010</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2012</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2013</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2015</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2008</t>
-  </si>
-  <si>
-    <t>Auto-updates (within IDE Extension Manager) occur successfully - VS2005</t>
   </si>
   <si>
     <r>
@@ -300,6 +282,12 @@
   </si>
   <si>
     <t>VS Gallery &amp; AppVeyor version numbers in sync</t>
+  </si>
+  <si>
+    <t>Auto-updates (within IDE Extension Manager) occur successfully (VS2015 &amp; above only)</t>
+  </si>
+  <si>
+    <t>When a rule exists for a project in a directory that is not within the solution file directory, it is still modified successfully</t>
   </si>
 </sst>
 </file>
@@ -680,13 +668,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -706,7 +694,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D1" s="2"/>
     </row>
@@ -1134,7 +1122,7 @@
         <v>30</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>0</v>
@@ -1145,7 +1133,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>0</v>
@@ -1156,7 +1144,7 @@
         <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>0</v>
@@ -1167,7 +1155,7 @@
         <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>0</v>
@@ -1177,8 +1165,8 @@
       <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>47</v>
+      <c r="B44" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>0</v>
@@ -1189,7 +1177,7 @@
         <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>0</v>
@@ -1200,7 +1188,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>0</v>
@@ -1211,7 +1199,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>0</v>
@@ -1222,10 +1210,10 @@
         <v>30</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>7</v>
+        <v>65</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1233,7 +1221,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>7</v>
@@ -1244,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
@@ -1255,10 +1243,10 @@
         <v>30</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1266,7 +1254,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>0</v>
@@ -1277,7 +1265,7 @@
         <v>30</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>0</v>
@@ -1285,10 +1273,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>0</v>
@@ -1299,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>0</v>
@@ -1310,7 +1298,7 @@
         <v>34</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>0</v>
@@ -1321,7 +1309,7 @@
         <v>34</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>0</v>
@@ -1332,7 +1320,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>0</v>
@@ -1343,7 +1331,7 @@
         <v>34</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>0</v>
@@ -1354,7 +1342,7 @@
         <v>34</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>0</v>
@@ -1365,7 +1353,7 @@
         <v>34</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>0</v>
@@ -1376,7 +1364,7 @@
         <v>34</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>0</v>
@@ -1387,7 +1375,7 @@
         <v>34</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>0</v>
@@ -1398,7 +1386,7 @@
         <v>34</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>0</v>
@@ -1406,10 +1394,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>0</v>
@@ -1420,7 +1408,7 @@
         <v>35</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>0</v>
@@ -1431,7 +1419,7 @@
         <v>35</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>0</v>
@@ -1442,7 +1430,7 @@
         <v>35</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>0</v>
@@ -1453,7 +1441,7 @@
         <v>35</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>0</v>
@@ -1464,7 +1452,7 @@
         <v>35</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>0</v>
@@ -1475,7 +1463,7 @@
         <v>35</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>0</v>
@@ -1483,10 +1471,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>0</v>
@@ -1497,7 +1485,7 @@
         <v>36</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>0</v>
@@ -1508,7 +1496,7 @@
         <v>36</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>0</v>
@@ -1519,7 +1507,7 @@
         <v>36</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>0</v>
@@ -1530,10 +1518,10 @@
         <v>36</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>7</v>
+        <v>62</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1541,10 +1529,10 @@
         <v>36</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>7</v>
+        <v>84</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1552,54 +1540,10 @@
         <v>36</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B79" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>7</v>
+      <c r="C78" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interim commit (untested) for git hub issue #2
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\autofindreplace\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="18510" windowHeight="13365"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="89">
   <si>
     <t>PASS</t>
   </si>
@@ -288,6 +283,15 @@
   </si>
   <si>
     <t>When a rule exists for a project in a directory that is not within the solution file directory, it is still modified successfully</t>
+  </si>
+  <si>
+    <t>GitHub contrib bar - move licence.txt up a level like filesforeverysuffix - add to test case.xls that it is on contrib bar--&gt;</t>
+  </si>
+  <si>
+    <t>GitHub contrib bar - github/linguist</t>
+  </si>
+  <si>
+    <t>GitHub contrib bar - website url (bit.ly)</t>
   </si>
 </sst>
 </file>
@@ -341,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -363,6 +367,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,7 +431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,7 +466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,13 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="B80" sqref="B80:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1546,6 +1553,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B79" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B80" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test case updates for license
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="88">
   <si>
     <t>PASS</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>LICENCE.txt is correct</t>
-  </si>
-  <si>
     <t>Manifest &gt; Installed Targets</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
   </si>
   <si>
     <t>GitHub ReadMe.md is generally okay</t>
-  </si>
-  <si>
-    <t>GitHub ReadMe.md LICENCE is okay</t>
   </si>
   <si>
     <t>GitHub ReadMe.md link to VS gallery is okay</t>
@@ -285,13 +279,16 @@
     <t>When a rule exists for a project in a directory that is not within the solution file directory, it is still modified successfully</t>
   </si>
   <si>
-    <t>GitHub contrib bar - move licence.txt up a level like filesforeverysuffix - add to test case.xls that it is on contrib bar--&gt;</t>
-  </si>
-  <si>
-    <t>GitHub contrib bar - github/linguist</t>
-  </si>
-  <si>
-    <t>GitHub contrib bar - website url (bit.ly)</t>
+    <t>LICENSE.txt is correct</t>
+  </si>
+  <si>
+    <t>GitHub ReadMe.md LICENSE.txt link is okay</t>
+  </si>
+  <si>
+    <t>GitHub contributors bar LICENSE link is okay</t>
+  </si>
+  <si>
+    <t>GitHub page title url for porject is a bit.ly link to the VS market place</t>
   </si>
 </sst>
 </file>
@@ -345,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -367,9 +364,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,13 +669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B80" sqref="B80:B81"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -695,22 +689,22 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -719,10 +713,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -730,10 +724,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -741,10 +735,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>0</v>
@@ -752,10 +746,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -763,10 +757,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>0</v>
@@ -774,7 +768,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
@@ -785,10 +779,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
@@ -796,10 +790,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>0</v>
@@ -807,10 +801,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>0</v>
@@ -818,10 +812,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>0</v>
@@ -829,10 +823,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>0</v>
@@ -840,10 +834,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
@@ -851,10 +845,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
@@ -862,10 +856,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
@@ -873,10 +867,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
@@ -884,10 +878,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
@@ -895,10 +889,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>0</v>
@@ -906,7 +900,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -917,7 +911,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>9</v>
@@ -928,7 +922,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>10</v>
@@ -939,7 +933,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>11</v>
@@ -950,10 +944,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>0</v>
@@ -961,7 +955,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>2</v>
@@ -972,10 +966,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>0</v>
@@ -983,10 +977,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>0</v>
@@ -994,10 +988,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>0</v>
@@ -1005,10 +999,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>0</v>
@@ -1016,10 +1010,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>0</v>
@@ -1027,10 +1021,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>0</v>
@@ -1038,10 +1032,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>0</v>
@@ -1049,10 +1043,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>0</v>
@@ -1060,10 +1054,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>0</v>
@@ -1071,10 +1065,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>0</v>
@@ -1082,10 +1076,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>0</v>
@@ -1093,10 +1087,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>0</v>
@@ -1104,10 +1098,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>0</v>
@@ -1115,10 +1109,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>0</v>
@@ -1126,10 +1120,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>0</v>
@@ -1137,10 +1131,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>0</v>
@@ -1148,10 +1142,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>0</v>
@@ -1159,10 +1153,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>0</v>
@@ -1170,10 +1164,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>0</v>
@@ -1181,10 +1175,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>0</v>
@@ -1192,10 +1186,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>0</v>
@@ -1203,10 +1197,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>0</v>
@@ -1214,10 +1208,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>0</v>
@@ -1225,10 +1219,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>7</v>
@@ -1236,10 +1230,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
@@ -1247,10 +1241,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>7</v>
@@ -1258,10 +1252,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>0</v>
@@ -1269,10 +1263,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>0</v>
@@ -1280,10 +1274,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>0</v>
@@ -1291,10 +1285,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>0</v>
@@ -1302,10 +1296,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>0</v>
@@ -1313,10 +1307,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>0</v>
@@ -1324,10 +1318,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>0</v>
@@ -1335,7 +1329,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>6</v>
@@ -1346,7 +1340,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
@@ -1357,10 +1351,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>0</v>
@@ -1368,7 +1362,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>4</v>
@@ -1379,7 +1373,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>3</v>
@@ -1390,10 +1384,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>0</v>
@@ -1401,10 +1395,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>0</v>
@@ -1412,10 +1406,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>0</v>
@@ -1423,10 +1417,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>0</v>
@@ -1434,10 +1428,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>0</v>
@@ -1445,10 +1439,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>0</v>
@@ -1456,10 +1450,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>0</v>
@@ -1467,10 +1461,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>0</v>
@@ -1478,10 +1472,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>0</v>
@@ -1489,10 +1483,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>0</v>
@@ -1500,10 +1494,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>0</v>
@@ -1511,10 +1505,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>0</v>
@@ -1522,10 +1516,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>0</v>
@@ -1533,10 +1527,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>0</v>
@@ -1544,28 +1538,35 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B79" s="8" t="s">
-        <v>88</v>
+      <c r="A79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B80" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="8" t="s">
-        <v>87</v>
+      <c r="A80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>